<commit_message>
Added graphs and stuff
</commit_message>
<xml_diff>
--- a/MESSAGEix_South_Africa/results/timeseries_SSP5_baseline.xlsx
+++ b/MESSAGEix_South_Africa/results/timeseries_SSP5_baseline.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jansn\GitHub\SSP5\MESSAGEix_South_Africa\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Documents/GitHub/SSP5/MESSAGEix_South_Africa/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF62E0-E45E-F847-8126-0836C063B182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1720" yWindow="460" windowWidth="24920" windowHeight="14400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CO2 emissions" sheetId="2" r:id="rId2"/>
+    <sheet name="Technology shares" sheetId="3" r:id="rId3"/>
+    <sheet name="Import Export" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">'Import Export'!$A$2:$B$2</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Import Export'!$A$3:$B$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Import Export'!$A$4:$B$4</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Import Export'!$C$1:$N$1</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Import Export'!$C$2:$N$2</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'Import Export'!$C$3:$N$3</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">'Import Export'!$C$4:$N$4</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="47">
   <si>
     <t>model</t>
   </si>
@@ -133,12 +146,39 @@
   </si>
   <si>
     <t>GW</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>RCP 1.9</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>RCP 2.6</t>
+  </si>
+  <si>
+    <t>RCP 3.4</t>
+  </si>
+  <si>
+    <t>RCP 4.5</t>
+  </si>
+  <si>
+    <t>RCP 6.0</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Exports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -187,15 +227,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,6 +268,2320 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Emissions [MtCO2eq]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RCP 1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RCP 2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RCP 3.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RCP 4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>RCP 6.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CO2 emissions'!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>527.53094482421875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-522A-9246-81E6-4B3D162E3457}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RCP 1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RCP 2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RCP 3.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RCP 4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>RCP 6.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CO2 emissions'!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>683.823974609375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>664.48138427734375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>664.48138427734375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>664.48138427734375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664.48138427734375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>664.48138427734375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-522A-9246-81E6-4B3D162E3457}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RCP 1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RCP 2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RCP 3.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RCP 4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>RCP 6.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CO2 emissions'!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>817.57855224609375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>744.68243408203125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>744.68243408203125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>744.68243408203125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>744.68243408203125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>744.68243408203125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-522A-9246-81E6-4B3D162E3457}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CO2 emissions'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RCP 1.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RCP 2.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RCP 3.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>RCP 4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>RCP 6.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CO2 emissions'!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1004.80712890625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>872.3360595703125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>872.3360595703125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>872.3360595703125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>872.3360595703125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>872.3360595703125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-522A-9246-81E6-4B3D162E3457}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="665126799"/>
+        <c:axId val="665081599"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="665126799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665081599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665081599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665126799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Trade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Import Export'!$A$3:$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Imports</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Import Export'!$C$1:$N$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Baseline</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>RCP 1.9</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>RCP 6.0</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Import Export'!$C$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>49.652545928955078</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.253894805908203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.423957824707031</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.234283447265618</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.652545928955078</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.902667999267578</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>48.413551330566413</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.411617279052727</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.652545928955078</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.902667999267578</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48.413551330566413</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.411617279052727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2B42-094F-A66F-4DF9A79C8691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Import Export'!$A$4:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Exports</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GWa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Import Export'!$C$1:$N$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2020</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2030</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2040</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2050</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Baseline</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>RCP 1.9</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>RCP 6.0</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Import Export'!$C$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>66.5994873046875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.925739288330078</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.783237457275391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.160850524902337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.5994873046875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.925739288330078</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.783237457275391</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44.160850524902337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.5994873046875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.925739288330078</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.783237457275391</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44.160850524902337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2B42-094F-A66F-4DF9A79C8691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="664870447"/>
+        <c:axId val="665500159"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="664870447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665500159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665500159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="664870447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F115C6C-1DC9-1847-80CB-7C5C839E4025}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF869289-E83F-E24E-8552-3B3AE0EA17CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -289,6 +2660,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -324,6 +2712,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,22 +2904,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="47.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +2948,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -575,7 +2980,7 @@
         <v>1004.80712890625</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -595,7 +3000,7 @@
         <v>36</v>
       </c>
       <c r="G3">
-        <v>33.254653930664063</v>
+        <v>33.254653930664062</v>
       </c>
       <c r="H3">
         <v>49.712669372558587</v>
@@ -607,7 +3012,7 @@
         <v>83.542770385742188</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -639,7 +3044,7 @@
         <v>148.26139831542969</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -671,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -703,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -735,7 +3140,7 @@
         <v>8.2092761993408203</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -755,10 +3160,10 @@
         <v>37</v>
       </c>
       <c r="G8">
-        <v>58.076187133789063</v>
+        <v>58.076187133789062</v>
       </c>
       <c r="H8">
-        <v>70.977310180664063</v>
+        <v>70.977310180664062</v>
       </c>
       <c r="I8">
         <v>48.583858489990227</v>
@@ -767,7 +3172,7 @@
         <v>126.8200225830078</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -799,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -831,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -863,7 +3268,7 @@
         <v>3.1300857663154602E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -895,7 +3300,7 @@
         <v>6.4623169600963593E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -927,7 +3332,7 @@
         <v>0.32006305456161499</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -947,7 +3352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -979,7 +3384,7 @@
         <v>12.90125560760498</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1011,7 +3416,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1043,7 +3448,7 @@
         <v>1.672427654266357</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1075,7 +3480,7 @@
         <v>0.7847975492477417</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1107,7 +3512,7 @@
         <v>9.2604048550128937E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1139,7 +3544,7 @@
         <v>9.5159310149028897E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1171,7 +3576,7 @@
         <v>0.82543516159057617</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1203,7 +3608,7 @@
         <v>9.7742579877376556E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1235,7 +3640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -1267,7 +3672,7 @@
         <v>306.140625</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1299,7 +3704,7 @@
         <v>306.44076538085938</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1331,7 +3736,7 @@
         <v>59.234283447265618</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -1363,7 +3768,7 @@
         <v>44.160850524902337</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -1398,4 +3803,756 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67452968-A60A-BD47-AD75-AF2085EA7817}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="C2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="D2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="E2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="F2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="G2">
+        <v>527.53094482421875</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2030</v>
+      </c>
+      <c r="B3">
+        <v>683.823974609375</v>
+      </c>
+      <c r="C3">
+        <v>664.48138427734375</v>
+      </c>
+      <c r="D3">
+        <v>664.48138427734375</v>
+      </c>
+      <c r="E3">
+        <v>664.48138427734375</v>
+      </c>
+      <c r="F3">
+        <v>664.48138427734375</v>
+      </c>
+      <c r="G3">
+        <v>664.48138427734375</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2040</v>
+      </c>
+      <c r="B4">
+        <v>817.57855224609375</v>
+      </c>
+      <c r="C4">
+        <v>744.68243408203125</v>
+      </c>
+      <c r="D4">
+        <v>744.68243408203125</v>
+      </c>
+      <c r="E4">
+        <v>744.68243408203125</v>
+      </c>
+      <c r="F4">
+        <v>744.68243408203125</v>
+      </c>
+      <c r="G4">
+        <v>744.68243408203125</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2050</v>
+      </c>
+      <c r="B5">
+        <v>1004.80712890625</v>
+      </c>
+      <c r="C5">
+        <v>872.3360595703125</v>
+      </c>
+      <c r="D5">
+        <v>872.3360595703125</v>
+      </c>
+      <c r="E5">
+        <v>872.3360595703125</v>
+      </c>
+      <c r="F5">
+        <v>872.3360595703125</v>
+      </c>
+      <c r="G5">
+        <v>872.3360595703125</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9E616C-D890-064D-BBE9-71133F42972D}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>33.254653930664062</v>
+      </c>
+      <c r="D3">
+        <v>49.712669372558587</v>
+      </c>
+      <c r="E3">
+        <v>68.00872802734375</v>
+      </c>
+      <c r="F3">
+        <v>83.542770385742188</v>
+      </c>
+      <c r="G3" s="5">
+        <v>33.254653930664062</v>
+      </c>
+      <c r="H3">
+        <v>48.202861785888672</v>
+      </c>
+      <c r="I3">
+        <v>61.804813385009773</v>
+      </c>
+      <c r="J3">
+        <v>71.801704406738281</v>
+      </c>
+      <c r="K3" s="5">
+        <v>33.254653930664062</v>
+      </c>
+      <c r="L3">
+        <v>48.202861785888672</v>
+      </c>
+      <c r="M3">
+        <v>61.804813385009773</v>
+      </c>
+      <c r="N3">
+        <v>71.801704406738281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>2.361545324325562</v>
+      </c>
+      <c r="D4">
+        <v>4.2988061904907227</v>
+      </c>
+      <c r="E4">
+        <v>5.9079771041870117</v>
+      </c>
+      <c r="F4">
+        <v>8.2092761993408203</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2.361545324325562</v>
+      </c>
+      <c r="H5">
+        <v>4.1944217681884766</v>
+      </c>
+      <c r="I5">
+        <v>5.4820828437805176</v>
+      </c>
+      <c r="J5">
+        <v>7.2296295166015616</v>
+      </c>
+      <c r="K5" s="5">
+        <v>2.361545324325562</v>
+      </c>
+      <c r="L5">
+        <v>4.1944217681884766</v>
+      </c>
+      <c r="M5">
+        <v>5.4820828437805176</v>
+      </c>
+      <c r="N5">
+        <v>7.2296295166015616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>0.73838180303573608</v>
+      </c>
+      <c r="D6">
+        <v>0.25745782256126398</v>
+      </c>
+      <c r="E6">
+        <v>8.9769989252090454E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.1300857663154602E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>0.28504565358161932</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4.1660981178283691</v>
+      </c>
+      <c r="F7">
+        <v>12.90125560760498</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.73838180303573608</v>
+      </c>
+      <c r="H7">
+        <v>0.25745782256126398</v>
+      </c>
+      <c r="I7">
+        <v>8.9769989252090454E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.1300857663154602E-2</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.73838180303573608</v>
+      </c>
+      <c r="L7">
+        <v>0.25745782256126398</v>
+      </c>
+      <c r="M7">
+        <v>8.9769989252090454E-2</v>
+      </c>
+      <c r="N7">
+        <v>3.1300857663154602E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>3.2628669738769531</v>
+      </c>
+      <c r="D8">
+        <v>4.4002127647399902</v>
+      </c>
+      <c r="E8">
+        <v>4.7964754104614258</v>
+      </c>
+      <c r="F8">
+        <v>1.672427654266357</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.28504565358161932</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>4.1660981178283691</v>
+      </c>
+      <c r="J8">
+        <v>12.90125560760498</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.28504565358161932</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>4.1660981178283691</v>
+      </c>
+      <c r="N8">
+        <v>12.90125560760498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>8.4144547581672668E-2</v>
+      </c>
+      <c r="D9">
+        <v>2.9339388012886051E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.023001223802567E-2</v>
+      </c>
+      <c r="F9">
+        <v>9.2604048550128937E-3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3.2628669738769531</v>
+      </c>
+      <c r="H9">
+        <v>4.4002127647399902</v>
+      </c>
+      <c r="I9">
+        <v>4.7964754104614258</v>
+      </c>
+      <c r="J9">
+        <v>1.672427654266357</v>
+      </c>
+      <c r="K9" s="5">
+        <v>3.2628669738769531</v>
+      </c>
+      <c r="L9">
+        <v>4.4002127647399902</v>
+      </c>
+      <c r="M9">
+        <v>4.7964754104614258</v>
+      </c>
+      <c r="N9">
+        <v>1.672427654266357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>1.2572259902954099</v>
+      </c>
+      <c r="D10">
+        <v>0.74865138530731201</v>
+      </c>
+      <c r="E10">
+        <v>0.79461699724197388</v>
+      </c>
+      <c r="F10">
+        <v>0.82543516159057617</v>
+      </c>
+      <c r="G10" s="5">
+        <v>8.4144547581672668E-2</v>
+      </c>
+      <c r="H10">
+        <v>2.9339388012886051E-2</v>
+      </c>
+      <c r="I10">
+        <v>1.023001223802567E-2</v>
+      </c>
+      <c r="J10">
+        <v>9.2604048550128937E-3</v>
+      </c>
+      <c r="K10" s="5">
+        <v>8.4144547581672668E-2</v>
+      </c>
+      <c r="L10">
+        <v>2.9339388012886051E-2</v>
+      </c>
+      <c r="M10">
+        <v>1.023001223802567E-2</v>
+      </c>
+      <c r="N10">
+        <v>9.2604048550128937E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G11" s="5">
+        <v>1.2572259902954099</v>
+      </c>
+      <c r="H11">
+        <v>0.74865138530731201</v>
+      </c>
+      <c r="I11">
+        <v>0.79461699724197388</v>
+      </c>
+      <c r="J11">
+        <v>0.82543516159057617</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1.2572259902954099</v>
+      </c>
+      <c r="L11">
+        <v>0.74865138530731201</v>
+      </c>
+      <c r="M11">
+        <v>0.79461699724197388</v>
+      </c>
+      <c r="N11">
+        <v>0.82543516159057617</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F7BD68-AF49-1D46-938F-BEF1C2D6638B}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2030</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2040</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2050</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2030</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2040</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2050</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2030</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2040</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3">
+        <v>49.652545928955078</v>
+      </c>
+      <c r="D3">
+        <v>47.253894805908203</v>
+      </c>
+      <c r="E3">
+        <v>53.423957824707031</v>
+      </c>
+      <c r="F3">
+        <v>59.234283447265618</v>
+      </c>
+      <c r="G3">
+        <v>49.652545928955078</v>
+      </c>
+      <c r="H3">
+        <v>45.902667999267578</v>
+      </c>
+      <c r="I3">
+        <v>48.413551330566413</v>
+      </c>
+      <c r="J3">
+        <v>49.411617279052727</v>
+      </c>
+      <c r="K3">
+        <v>49.652545928955078</v>
+      </c>
+      <c r="L3">
+        <v>45.902667999267578</v>
+      </c>
+      <c r="M3">
+        <v>48.413551330566413</v>
+      </c>
+      <c r="N3">
+        <v>49.411617279052727</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>66.5994873046875</v>
+      </c>
+      <c r="D4">
+        <v>52.925739288330078</v>
+      </c>
+      <c r="E4">
+        <v>46.783237457275391</v>
+      </c>
+      <c r="F4">
+        <v>44.160850524902337</v>
+      </c>
+      <c r="G4">
+        <v>66.5994873046875</v>
+      </c>
+      <c r="H4">
+        <v>52.925739288330078</v>
+      </c>
+      <c r="I4">
+        <v>46.783237457275391</v>
+      </c>
+      <c r="J4">
+        <v>44.160850524902337</v>
+      </c>
+      <c r="K4">
+        <v>66.5994873046875</v>
+      </c>
+      <c r="L4">
+        <v>52.925739288330078</v>
+      </c>
+      <c r="M4">
+        <v>46.783237457275391</v>
+      </c>
+      <c r="N4">
+        <v>44.160850524902337</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>